<commit_message>
updated classification results saving, template.xlsx, and User Guide.docx
1) Classification results are now saved as "Good"/"Usable"/"Noise" instead of 1/2/3.

2) Visual formatting of results has been updated in template.xlsx. Easier to see what goes well/wrong in Results.xlsx through color coding.

3) Added Limitations section to User Guide.docx and updated Input/Output sections.

4) Setup .xml template is now appropriately named autoC3Dsetup.xml.
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Melbourne ACLR Dataset\_Sorted Gait Data\_Auto C3D Checker\_Git Version\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB5F063-A746-4ACA-9E4C-A43EC655B862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1510EE0C-ACA5-4F3F-948C-CF21C4BE25CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4762983E-9798-4FFD-8541-0981FAB3A3BF}"/>
   </bookViews>
@@ -63,7 +63,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -73,6 +73,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -119,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -133,25 +139,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="36">
     <dxf>
       <border>
         <left style="thin">
@@ -173,6 +168,118 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="1"/>
         </patternFill>
       </fill>
@@ -196,35 +303,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
         </patternFill>
       </fill>
     </dxf>
@@ -249,6 +328,111 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="1"/>
         </patternFill>
       </fill>
@@ -268,27 +452,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -605,23 +768,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A98E2CE-6566-4EDB-9C88-3A10A55AA703}">
-  <dimension ref="A1:BA51"/>
+  <dimension ref="A1:CZ51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="53" width="13.28515625" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="22.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="104" width="13.28515625" style="1" customWidth="1"/>
+    <col min="105" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:104" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -679,8 +842,59 @@
       <c r="AY1" s="4"/>
       <c r="AZ1" s="4"/>
       <c r="BA1" s="4"/>
+      <c r="BB1" s="4"/>
+      <c r="BC1" s="4"/>
+      <c r="BD1" s="4"/>
+      <c r="BE1" s="4"/>
+      <c r="BF1" s="4"/>
+      <c r="BG1" s="4"/>
+      <c r="BH1" s="4"/>
+      <c r="BI1" s="4"/>
+      <c r="BJ1" s="4"/>
+      <c r="BK1" s="4"/>
+      <c r="BL1" s="4"/>
+      <c r="BM1" s="4"/>
+      <c r="BN1" s="4"/>
+      <c r="BO1" s="4"/>
+      <c r="BP1" s="4"/>
+      <c r="BQ1" s="4"/>
+      <c r="BR1" s="4"/>
+      <c r="BS1" s="4"/>
+      <c r="BT1" s="4"/>
+      <c r="BU1" s="4"/>
+      <c r="BV1" s="4"/>
+      <c r="BW1" s="4"/>
+      <c r="BX1" s="4"/>
+      <c r="BY1" s="4"/>
+      <c r="BZ1" s="4"/>
+      <c r="CA1" s="4"/>
+      <c r="CB1" s="4"/>
+      <c r="CC1" s="4"/>
+      <c r="CD1" s="4"/>
+      <c r="CE1" s="4"/>
+      <c r="CF1" s="4"/>
+      <c r="CG1" s="4"/>
+      <c r="CH1" s="4"/>
+      <c r="CI1" s="4"/>
+      <c r="CJ1" s="4"/>
+      <c r="CK1" s="4"/>
+      <c r="CL1" s="4"/>
+      <c r="CM1" s="4"/>
+      <c r="CN1" s="4"/>
+      <c r="CO1" s="4"/>
+      <c r="CP1" s="4"/>
+      <c r="CQ1" s="4"/>
+      <c r="CR1" s="4"/>
+      <c r="CS1" s="4"/>
+      <c r="CT1" s="4"/>
+      <c r="CU1" s="4"/>
+      <c r="CV1" s="4"/>
+      <c r="CW1" s="4"/>
+      <c r="CX1" s="4"/>
+      <c r="CY1" s="4"/>
+      <c r="CZ1" s="4"/>
     </row>
-    <row r="2" spans="1:53" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:104" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="25:25" x14ac:dyDescent="0.25">
       <c r="Y49" s="2"/>
     </row>
@@ -691,29 +905,62 @@
       <c r="Y51" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:BA1048576">
-    <cfRule type="expression" dxfId="6" priority="1">
+  <conditionalFormatting sqref="A2:CZ1048576">
+    <cfRule type="containsBlanks" dxfId="35" priority="1" stopIfTrue="1">
+      <formula>LEN(TRIM(A2))=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="6" stopIfTrue="1">
+      <formula>IF(AND(A$1="Trial Usability",A2="Calibration"),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="7" stopIfTrue="1">
+      <formula>IF(AND(A$1="Trial Usability",A2="Execution"),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="8" stopIfTrue="1">
       <formula>IF(AND(A$1="Trial Usability",A2="Unusable"),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2">
-      <formula>IF(AND(A$1="Trial Usability",A2="Execution"),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="3">
-      <formula>IF(AND(A$1="Trial Usability",A2="Calibration"),TRUE,FALSE)</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="3" priority="8" stopIfTrue="1">
-      <formula>LEN(TRIM(A2))=0</formula>
+    <cfRule type="expression" dxfId="31" priority="9">
+      <formula>IF(AND(A$1="Instrumented Leg Hit FP?",A2="Yes"),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="10">
+      <formula>IF(AND(A$1="Instrumented Leg Hit FP?",A2="No"),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="11" stopIfTrue="1">
+      <formula>IF(AND(A$1="Percentage Usable EMG",AND(NOT(ISBLANK(A2)),A2&lt;50)),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="12" stopIfTrue="1">
+      <formula>IF(AND(A$1="Percentage Usable EMG",AND(A2&lt;75,A2&gt;49.99)),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="13" stopIfTrue="1">
+      <formula>IF(AND(A$1="Percentage Usable EMG",A2&gt;74.99),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="14" operator="containsText" text="Noise">
+      <formula>NOT(ISERROR(SEARCH("Noise",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="19" operator="containsText" text="Usable">
+      <formula>NOT(ISERROR(SEARCH("Usable",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="20" operator="containsText" text="Good">
+      <formula>NOT(ISERROR(SEARCH("Good",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="Artefact">
+      <formula>NOT(ISERROR(SEARCH("Artefact",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="64" operator="containsText" text="Error">
+      <formula>NOT(ISERROR(SEARCH("Error",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="3" stopIfTrue="1" operator="containsText" text="Calibration">
+      <formula>NOT(ISERROR(SEARCH("Calibration",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="4" stopIfTrue="1" operator="containsText" text="Execution">
+      <formula>NOT(ISERROR(SEARCH("Execution",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="5" stopIfTrue="1" operator="containsText" text="Unusable">
+      <formula>NOT(ISERROR(SEARCH("Unusable",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:BA1048576">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="9">
+  <conditionalFormatting sqref="B2:CZ1048576">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="10" stopIfTrue="1" operator="containsText" text="Artefact">
-      <formula>NOT(ISERROR(SEARCH("Artefact",B2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="53" operator="containsText" text="Error">
-      <formula>NOT(ISERROR(SEARCH("Error",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New lastFrame, MVC envelopes, and elaboration bonus script
1) Added MVC envelope calculation from all trials.

2) Added lastFrame for trials where subject remains on the FP until the end of the trial.

3) Added bonus script for automated generation of elaboration.xml.
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Melbourne ACLR Dataset\_Sorted Gait Data\_Auto C3D Checker\_Git Version\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1510EE0C-ACA5-4F3F-948C-CF21C4BE25CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7ABEABF-C892-41EA-9468-5FC54F2D3EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4762983E-9798-4FFD-8541-0981FAB3A3BF}"/>
   </bookViews>
@@ -34,12 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Trials</t>
   </si>
   <si>
     <t>Instrumented Leg</t>
+  </si>
+  <si>
+    <t>Instrumented Leg Hit FP?</t>
   </si>
 </sst>
 </file>
@@ -146,7 +149,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="19">
     <dxf>
       <border>
         <left style="thin">
@@ -168,6 +171,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF8181"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="5"/>
         </patternFill>
       </fill>
@@ -175,6 +206,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -182,6 +220,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
@@ -189,14 +241,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -210,6 +262,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -217,218 +276,12 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <fill>
@@ -771,10 +624,10 @@
   <dimension ref="A1:CZ51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,7 +644,9 @@
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
@@ -906,60 +761,63 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:CZ1048576">
-    <cfRule type="containsBlanks" dxfId="35" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="18" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="3">
+      <formula>IF(COUNTIF(A$1,"Max_*"),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="4" stopIfTrue="1" operator="containsText" text="Calibration">
+      <formula>NOT(ISERROR(SEARCH("Calibration",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="5" stopIfTrue="1" operator="containsText" text="Execution">
+      <formula>NOT(ISERROR(SEARCH("Execution",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="6" stopIfTrue="1" operator="containsText" text="Unusable">
+      <formula>NOT(ISERROR(SEARCH("Unusable",A2)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="7" stopIfTrue="1">
       <formula>IF(AND(A$1="Trial Usability",A2="Calibration"),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="8" stopIfTrue="1">
       <formula>IF(AND(A$1="Trial Usability",A2="Execution"),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="9" stopIfTrue="1">
       <formula>IF(AND(A$1="Trial Usability",A2="Unusable"),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="9">
+    <cfRule type="expression" dxfId="10" priority="10">
       <formula>IF(AND(A$1="Instrumented Leg Hit FP?",A2="Yes"),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="10">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>IF(AND(A$1="Instrumented Leg Hit FP?",A2="No"),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="12" stopIfTrue="1">
       <formula>IF(AND(A$1="Percentage Usable EMG",AND(NOT(ISBLANK(A2)),A2&lt;50)),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="13" stopIfTrue="1">
       <formula>IF(AND(A$1="Percentage Usable EMG",AND(A2&lt;75,A2&gt;49.99)),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="14" stopIfTrue="1">
       <formula>IF(AND(A$1="Percentage Usable EMG",A2&gt;74.99),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="14" operator="containsText" text="Noise">
+    <cfRule type="containsText" dxfId="5" priority="15" operator="containsText" text="Noise">
       <formula>NOT(ISERROR(SEARCH("Noise",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="19" operator="containsText" text="Usable">
+    <cfRule type="containsText" dxfId="4" priority="20" operator="containsText" text="Usable">
       <formula>NOT(ISERROR(SEARCH("Usable",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="20" operator="containsText" text="Good">
+    <cfRule type="containsText" dxfId="3" priority="21" operator="containsText" text="Good">
       <formula>NOT(ISERROR(SEARCH("Good",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="Artefact">
+    <cfRule type="containsText" dxfId="2" priority="22" operator="containsText" text="Artefact">
       <formula>NOT(ISERROR(SEARCH("Artefact",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="64" operator="containsText" text="Error">
+    <cfRule type="containsText" dxfId="1" priority="65" operator="containsText" text="Error">
       <formula>NOT(ISERROR(SEARCH("Error",A2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="3" stopIfTrue="1" operator="containsText" text="Calibration">
-      <formula>NOT(ISERROR(SEARCH("Calibration",A2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="4" stopIfTrue="1" operator="containsText" text="Execution">
-      <formula>NOT(ISERROR(SEARCH("Execution",A2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="5" stopIfTrue="1" operator="containsText" text="Unusable">
-      <formula>NOT(ISERROR(SEARCH("Unusable",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:CZ1048576">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>